<commit_message>
Update Excel scopes in working document
</commit_message>
<xml_diff>
--- a/Vinnusvæði/Authentication/UseCaseDraft.xlsx
+++ b/Vinnusvæði/Authentication/UseCaseDraft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\KS-IST-FUT-FMTH\Vinnusvæði\Authentication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A48CE33-AB32-494E-849A-8A1F77A52D84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C805AA-155E-42F7-8AEF-510508DACDE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="47565" windowHeight="18450" xr2:uid="{9CEF9921-4C1E-493D-A720-ED88E3B58C2F}"/>
+    <workbookView xWindow="5235" yWindow="540" windowWidth="39105" windowHeight="18450" xr2:uid="{9CEF9921-4C1E-493D-A720-ED88E3B58C2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="108">
   <si>
     <t xml:space="preserve">IOBWS3.0.yaml:98:           </t>
   </si>
@@ -344,12 +344,6 @@
     <t>ais:{consentId}</t>
   </si>
   <si>
-    <t>cur.read</t>
-  </si>
-  <si>
-    <t>cts.read, cts.write</t>
-  </si>
-  <si>
     <t>ccs.read, ccs.write</t>
   </si>
   <si>
@@ -357,6 +351,12 @@
   </si>
   <si>
     <t>doc.read, doc.write</t>
+  </si>
+  <si>
+    <t>doc.read</t>
+  </si>
+  <si>
+    <t>cts.read</t>
   </si>
 </sst>
 </file>
@@ -723,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D2CBD7C-2D6B-4B3C-B1DA-63517CD49C6B}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,9 +987,6 @@
       <c r="B23" t="s">
         <v>70</v>
       </c>
-      <c r="C23" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -998,9 +995,6 @@
       <c r="B24" t="s">
         <v>71</v>
       </c>
-      <c r="C24" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1009,9 +1003,6 @@
       <c r="B25" t="s">
         <v>72</v>
       </c>
-      <c r="C25" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1020,9 +1011,6 @@
       <c r="B26" t="s">
         <v>73</v>
       </c>
-      <c r="C26" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1031,9 +1019,6 @@
       <c r="B27" t="s">
         <v>74</v>
       </c>
-      <c r="C27" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1043,7 +1028,7 @@
         <v>75</v>
       </c>
       <c r="C28" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1054,7 +1039,7 @@
         <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1065,7 +1050,7 @@
         <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1076,7 +1061,7 @@
         <v>78</v>
       </c>
       <c r="C31" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1087,7 +1072,7 @@
         <v>79</v>
       </c>
       <c r="C32" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1098,7 +1083,7 @@
         <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1109,7 +1094,7 @@
         <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1119,6 +1104,9 @@
       <c r="B35" t="s">
         <v>82</v>
       </c>
+      <c r="C35" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
@@ -1127,6 +1115,9 @@
       <c r="B36" t="s">
         <v>83</v>
       </c>
+      <c r="C36" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -1135,6 +1126,9 @@
       <c r="B37" t="s">
         <v>84</v>
       </c>
+      <c r="C37" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -1143,6 +1137,9 @@
       <c r="B38" t="s">
         <v>85</v>
       </c>
+      <c r="C38" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -1151,6 +1148,9 @@
       <c r="B39" t="s">
         <v>86</v>
       </c>
+      <c r="C39" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
@@ -1159,6 +1159,9 @@
       <c r="B40" t="s">
         <v>87</v>
       </c>
+      <c r="C40" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -1167,6 +1170,9 @@
       <c r="B41" t="s">
         <v>88</v>
       </c>
+      <c r="C41" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -1175,6 +1181,9 @@
       <c r="B42" t="s">
         <v>89</v>
       </c>
+      <c r="C42" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -1183,6 +1192,9 @@
       <c r="B43" t="s">
         <v>90</v>
       </c>
+      <c r="C43" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -1191,6 +1203,9 @@
       <c r="B44" t="s">
         <v>91</v>
       </c>
+      <c r="C44" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -1199,6 +1214,9 @@
       <c r="B45" t="s">
         <v>92</v>
       </c>
+      <c r="C45" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
@@ -1207,6 +1225,9 @@
       <c r="B46" t="s">
         <v>93</v>
       </c>
+      <c r="C46" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -1216,7 +1237,7 @@
         <v>94</v>
       </c>
       <c r="C47" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1227,7 +1248,7 @@
         <v>95</v>
       </c>
       <c r="C48" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1238,7 +1259,7 @@
         <v>96</v>
       </c>
       <c r="C49" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>